<commit_message>
test git adjust dsach
</commit_message>
<xml_diff>
--- a/DanhSachNhom.xlsx
+++ b/DanhSachNhom.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IUH\Ki7\PTUD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\N4_HK1\PTUD\baitalon\PTUD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3078229-9A56-4551-A2D6-F0A14AD3CB99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2385" yWindow="4740" windowWidth="21600" windowHeight="11385" xr2:uid="{FDDD70FB-E348-436C-9966-EDEAB7A78336}"/>
+    <workbookView xWindow="2385" yWindow="4740" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -63,16 +62,16 @@
     <t>Lương Thị</t>
   </si>
   <si>
-    <t>Thu</t>
-  </si>
-  <si>
     <t>Nhóm trưởng</t>
+  </si>
+  <si>
+    <t>Thuu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -139,13 +138,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -460,11 +459,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B67544-4F2F-4DC1-AC8C-D95495122850}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="I4:J4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,13 +508,13 @@
       <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
       <c r="H5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -525,14 +524,14 @@
       <c r="C6" s="2">
         <v>17025241</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -542,14 +541,14 @@
       <c r="C7" s="2">
         <v>17024881</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
       <c r="H7" s="2"/>
     </row>
   </sheetData>

</xml_diff>